<commit_message>
add index for list tag
</commit_message>
<xml_diff>
--- a/labs/test-onetwo/src/test/resources/org/onetwo/common/excel/excel-template.xlsx
+++ b/labs/test-onetwo/src/test/resources/org/onetwo/common/excel/excel-template.xlsx
@@ -147,15 +147,15 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>[row:list datalist as data]</t>
+    <t>${totalLabel}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[row:list datalist as data, index]</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>${totalLabel}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>${data.id}</t>
+    <t>${index}</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -428,6 +428,51 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -436,51 +481,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -795,7 +795,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:B6"/>
+      <selection activeCell="A7" sqref="A7:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -810,10 +810,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="9"/>
+      <c r="B1" s="24"/>
     </row>
     <row r="2" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="28" t="s">
@@ -833,30 +833,30 @@
       <c r="B3" s="27"/>
       <c r="C3" s="27"/>
       <c r="D3" s="27"/>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
     </row>
     <row r="4" spans="1:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="11" t="s">
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
     </row>
     <row r="5" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="13"/>
+      <c r="B5" s="10"/>
       <c r="C5" s="3" t="s">
         <v>2</v>
       </c>
@@ -874,10 +874,10 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="13"/>
+      <c r="A6" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="10"/>
       <c r="C6" s="8"/>
       <c r="D6" s="7"/>
       <c r="E6" s="1"/>
@@ -887,10 +887,10 @@
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="13"/>
+      <c r="B7" s="10"/>
       <c r="C7" s="8" t="s">
         <v>16</v>
       </c>
@@ -902,10 +902,10 @@
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="13"/>
+      <c r="B8" s="10"/>
       <c r="C8" s="8"/>
       <c r="D8" s="7"/>
       <c r="E8" s="1"/>
@@ -915,10 +915,10 @@
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="13"/>
+      <c r="A9" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="10"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1">
@@ -934,41 +934,41 @@
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="116.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
     </row>
     <row r="11" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="19"/>
-      <c r="B11" s="21" t="s">
+      <c r="A11" s="16"/>
+      <c r="B11" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="21" t="s">
+      <c r="C11" s="19"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="22"/>
-      <c r="G11" s="23"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="20"/>
     </row>
     <row r="12" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="20"/>
-      <c r="B12" s="24" t="s">
+      <c r="A12" s="17"/>
+      <c r="B12" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="24" t="s">
+      <c r="C12" s="22"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="25"/>
-      <c r="G12" s="26"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="18">
@@ -977,6 +977,11 @@
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="E4:G4"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="E10:G10"/>
@@ -985,11 +990,6 @@
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="E11:G11"/>
     <mergeCell ref="E12:G12"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A7:B7"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>